<commit_message>
fingercap in M4-M4 test
</commit_message>
<xml_diff>
--- a/mag/adc_array_topologies/overview.xlsx
+++ b/mag/adc_array_topologies/overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28b581510f85c979/Studium/_Masterarbeit/eda/designs/SKY130_SAR-ADC/mag/adc_array_topologies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{EC155394-F565-4A08-89D8-1AF8DCF4F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F321642-9F17-47AD-BEB3-6A89C856484E}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{EC155394-F565-4A08-89D8-1AF8DCF4F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9F2D9A-6ABC-4FC9-BCE8-3A2E391FDD62}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{0DF55CA2-8073-418B-B7FF-723FBF917B41}"/>
+    <workbookView xWindow="8295" yWindow="2625" windowWidth="20550" windowHeight="11835" xr2:uid="{0DF55CA2-8073-418B-B7FF-723FBF917B41}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Waffle A (16)</t>
   </si>
@@ -132,6 +132,21 @@
   </si>
   <si>
     <t>1cell unitcap</t>
+  </si>
+  <si>
+    <t>Finger (8) F</t>
+  </si>
+  <si>
+    <t>M4-M4</t>
+  </si>
+  <si>
+    <t>Unit-Cap Mittelwert</t>
+  </si>
+  <si>
+    <t>Bin-Cap Berechnung</t>
+  </si>
+  <si>
+    <t>Gesamt-Cap</t>
   </si>
 </sst>
 </file>
@@ -139,11 +154,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.00&quot;fF&quot;"/>
-    <numFmt numFmtId="170" formatCode="0.00&quot;aF&quot;"/>
-    <numFmt numFmtId="171" formatCode="0&quot;um²&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.00&quot;fF&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.00&quot;aF&quot;"/>
+    <numFmt numFmtId="166" formatCode="0&quot;um²&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +187,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,33 +216,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -243,13 +267,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>78628</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -257,7 +281,7 @@
         <xdr:cNvPr id="2" name="Grafik 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{383F3576-510A-07AF-B3B7-D1A424EBAD8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -294,13 +318,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>86127</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -308,7 +332,7 @@
         <xdr:cNvPr id="3" name="Grafik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D30DFCAF-867F-14A2-EE7E-F630D5C9914F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -338,13 +362,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>114700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -352,7 +376,7 @@
         <xdr:cNvPr id="4" name="Grafik 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A2F74F9-BC2A-28BC-A804-DEC83C69C9CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -384,13 +408,13 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>26</xdr:row>
+          <xdr:row>29</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1000584</xdr:colOff>
-          <xdr:row>34</xdr:row>
+          <xdr:colOff>1000125</xdr:colOff>
+          <xdr:row>37</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -401,7 +425,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF1A084F-CD2C-CFFE-C766-BF52A2F24CED}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -436,13 +460,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1019175</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>156594</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -450,7 +474,7 @@
         <xdr:cNvPr id="5" name="Grafik 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2DC2EB6-41B1-021F-2DB1-C4463D10E16E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -480,13 +504,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9843</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>18734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>171931</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -494,7 +518,7 @@
         <xdr:cNvPr id="6" name="Grafik 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8120076-8779-F744-2721-6F3F344FA0A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -524,13 +548,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>2555</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -538,7 +562,7 @@
         <xdr:cNvPr id="7" name="Grafik 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC8D9F8-21E8-330F-35BB-DDBCF9FB8401}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -556,6 +580,50 @@
         <a:xfrm>
           <a:off x="7372350" y="2667001"/>
           <a:ext cx="1050305" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Grafik 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE5B1E6-6EF0-BE7E-F035-39E8ECA89C0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420101" y="5553076"/>
+          <a:ext cx="1066799" cy="1723926"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -864,19 +932,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDFAB4B-C293-46AC-B464-F4C2784181A4}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -901,8 +970,11 @@
       <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -927,8 +999,11 @@
       <c r="H2" s="8">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -953,8 +1028,11 @@
       <c r="H3" s="2">
         <v>5.55</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>4.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -979,441 +1057,476 @@
       <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>54.98</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
         <v>4.42</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
         <v>59.74</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>28.51</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <v>3.66</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>18.690000000000001</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>4.83</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="2">
         <v>6.43</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H8" s="2">
         <v>33.340000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="I8" s="2">
+        <v>29.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>57.53</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>30.99</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2">
-        <v>20.23</v>
-      </c>
-      <c r="F8" s="2">
-        <v>4.72</v>
-      </c>
-      <c r="G8" s="2">
-        <v>7.12</v>
-      </c>
-      <c r="H8" s="2">
-        <v>36.159999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2">
-        <v>56.42</v>
-      </c>
-      <c r="C9" s="2">
-        <v>29.86</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="2">
+        <v>20.23</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4.72</v>
+      </c>
+      <c r="G9" s="2">
+        <v>7.12</v>
+      </c>
+      <c r="H9" s="2">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="I9" s="2">
+        <v>32.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>56.42</v>
+      </c>
+      <c r="C10" s="2">
+        <v>29.86</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="2">
         <v>19.510000000000002</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <v>4.68</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <v>6.91</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <v>34.909999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="I10" s="2">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>55.85</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>29.29</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="4">
         <v>0.7</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <v>19.13</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>4.66</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <v>6.78</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <v>34.299999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="I11" s="2">
+        <v>30.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B14" s="3">
         <v>573</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
         <v>46</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B15" s="3">
         <v>574</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C15" s="3">
         <v>594</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D15" s="6">
         <v>457</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E15" s="3">
         <v>389</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F15" s="3">
         <v>46.4</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G15" s="3">
         <v>134</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H15" s="3">
         <v>694.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="I15" s="3">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B16" s="3">
         <v>575</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C16" s="3">
         <v>596</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="3">
+      <c r="D16" s="6"/>
+      <c r="E16" s="3">
         <v>389</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F16" s="3">
         <v>47.2</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G16" s="3">
         <v>136.9</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H16" s="3">
         <v>695.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="I16" s="3">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B17" s="3">
         <v>576</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C17" s="3">
         <v>597</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="3">
+      <c r="D17" s="6"/>
+      <c r="E17" s="3">
         <v>390</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F17" s="3">
         <v>47.8</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G17" s="3">
         <v>138.19999999999999</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H17" s="3">
         <v>698.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="I17" s="3">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B18" s="3">
         <v>576</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C18" s="3">
         <v>598</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D18" s="6">
         <v>700</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E18" s="3">
         <v>390</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F18" s="3">
         <v>48</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G18" s="3">
         <v>138.4</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H18" s="3">
         <v>700</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="I18" s="3">
+        <v>623.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3">
-        <f>B6/6/16*1000</f>
+      <c r="B21" s="3">
+        <f>B7/6/16*1000</f>
         <v>572.70833333333326</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3">
-        <f>F6/6/16*1000</f>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <f>F7/6/16*1000</f>
         <v>46.041666666666671</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="3">
-        <f>(B7-B$6)/8*1000</f>
+      <c r="B22" s="3">
+        <f>(B8-B$7)/8*1000</f>
         <v>595.00000000000068</v>
       </c>
-      <c r="C19" s="3">
-        <f>C7/6/8*1000</f>
+      <c r="C22" s="3">
+        <f>C8/6/8*1000</f>
         <v>593.95833333333337</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3">
-        <f>E7/6/8*1000</f>
-        <v>389.375</v>
-      </c>
-      <c r="F19" s="6">
-        <f t="shared" ref="C19:H19" si="0">(F7-F$6)/8*1000</f>
-        <v>51.250000000000014</v>
-      </c>
-      <c r="G19" s="6">
-        <f>G7/6/8*1000</f>
-        <v>133.95833333333331</v>
-      </c>
-      <c r="H19" s="3">
-        <f>H7/6/8*1000</f>
-        <v>694.58333333333348</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="3">
-        <f>(B8-B$6)/4*1000</f>
-        <v>637.50000000000102</v>
-      </c>
-      <c r="C20" s="3">
-        <f>(C8-C$7)/4*1000</f>
-        <v>619.9999999999992</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3">
-        <f>(E8-E$7)/4*1000</f>
-        <v>384.99999999999977</v>
-      </c>
-      <c r="F20" s="6">
-        <f t="shared" ref="C20:H20" si="1">(F8-F$6)/4*1000</f>
-        <v>74.999999999999957</v>
-      </c>
-      <c r="G20" s="6">
-        <f>(G8-G$7)/4*1000</f>
-        <v>172.50000000000009</v>
-      </c>
-      <c r="H20" s="3">
-        <f>(H8-H$7)/4*1000</f>
-        <v>704.99999999999829</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="3">
-        <f>(B9-B$6)/2*1000</f>
-        <v>720.00000000000239</v>
-      </c>
-      <c r="C21" s="3">
-        <f>(C9-C$7)/2*1000</f>
-        <v>674.99999999999898</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3">
-        <f>(E9-E$7)/2*1000</f>
-        <v>410.00000000000011</v>
-      </c>
-      <c r="F21" s="6">
-        <f>(F9-F$6)/2*1000</f>
-        <v>129.99999999999989</v>
-      </c>
-      <c r="G21" s="6">
-        <f>(G9-G$7)/2*1000</f>
-        <v>240.00000000000023</v>
-      </c>
-      <c r="H21" s="3">
-        <f>(H9-H$7)/2*1000</f>
-        <v>784.99999999999659</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="3">
-        <f>(B10-B$6)/1*1000</f>
-        <v>870.00000000000455</v>
-      </c>
-      <c r="C22" s="3">
-        <f>(C10-C$7)/1*1000</f>
-        <v>779.99999999999761</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3">
-        <f>(E10-E$7)/1*1000</f>
+        <f>E8/6/8*1000</f>
+        <v>389.375</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" ref="F22" si="0">(F8-F$7)/8*1000</f>
+        <v>51.250000000000014</v>
+      </c>
+      <c r="G22" s="6">
+        <f>G8/6/8*1000</f>
+        <v>133.95833333333331</v>
+      </c>
+      <c r="H22" s="3">
+        <f>H8/6/8*1000</f>
+        <v>694.58333333333348</v>
+      </c>
+      <c r="I22" s="3">
+        <f>I8/6/8*1000</f>
+        <v>621.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3">
+        <f>(B9-B$7)/4*1000</f>
+        <v>637.50000000000102</v>
+      </c>
+      <c r="C23" s="3">
+        <f>(C9-C$8)/4*1000</f>
+        <v>619.9999999999992</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
+        <f>(E9-E$8)/4*1000</f>
+        <v>384.99999999999977</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" ref="F23" si="1">(F9-F$7)/4*1000</f>
+        <v>74.999999999999957</v>
+      </c>
+      <c r="G23" s="6">
+        <f>(G9-G$8)/4*1000</f>
+        <v>172.50000000000009</v>
+      </c>
+      <c r="H23" s="3">
+        <f>(H9-H$8)/4*1000</f>
+        <v>704.99999999999829</v>
+      </c>
+      <c r="I23" s="3">
+        <f>(I9-I$8)/4*1000</f>
+        <v>642.50000000000011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3">
+        <f>(B10-B$7)/2*1000</f>
+        <v>720.00000000000239</v>
+      </c>
+      <c r="C24" s="3">
+        <f>(C10-C$8)/2*1000</f>
+        <v>674.99999999999898</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3">
+        <f>(E10-E$8)/2*1000</f>
+        <v>410.00000000000011</v>
+      </c>
+      <c r="F24" s="6">
+        <f>(F10-F$7)/2*1000</f>
+        <v>129.99999999999989</v>
+      </c>
+      <c r="G24" s="6">
+        <f>(G10-G$8)/2*1000</f>
+        <v>240.00000000000023</v>
+      </c>
+      <c r="H24" s="3">
+        <f>(H10-H$8)/2*1000</f>
+        <v>784.99999999999659</v>
+      </c>
+      <c r="I24" s="3">
+        <f>(I10-I$8)/2*1000</f>
+        <v>689.99999999999955</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="3">
+        <f>(B11-B$7)/1*1000</f>
+        <v>870.00000000000455</v>
+      </c>
+      <c r="C25" s="3">
+        <f>(C11-C$8)/1*1000</f>
+        <v>779.99999999999761</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3">
+        <f>(E11-E$8)/1*1000</f>
         <v>439.99999999999773</v>
       </c>
-      <c r="F22" s="6">
-        <f>(F10-F$6)/1*1000</f>
+      <c r="F25" s="6">
+        <f>(F11-F$7)/1*1000</f>
         <v>240.00000000000023</v>
       </c>
-      <c r="G22" s="6">
-        <f>(G10-G$7)/1*1000</f>
+      <c r="G25" s="6">
+        <f>(G11-G$8)/1*1000</f>
         <v>350.00000000000051</v>
       </c>
-      <c r="H22" s="3">
-        <f>(H10-H$7)/1*1000</f>
+      <c r="H25" s="3">
+        <f>(H11-H$8)/1*1000</f>
         <v>959.99999999999375</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="3">
+        <f>(I11-I$8)/1*1000</f>
+        <v>730.00000000000045</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="6"/>
@@ -1421,6 +1534,43 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1436,13 +1586,13 @@
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>1000125</xdr:colOff>
-                <xdr:row>34</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>

</xml_diff>

<commit_message>
comparable layout, bin caps on bottom
</commit_message>
<xml_diff>
--- a/mag/adc_array_topologies/overview.xlsx
+++ b/mag/adc_array_topologies/overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28b581510f85c979/Studium/_Masterarbeit/eda/designs/SKY130_SAR-ADC/mag/adc_array_topologies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{EC155394-F565-4A08-89D8-1AF8DCF4F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9F2D9A-6ABC-4FC9-BCE8-3A2E391FDD62}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{EC155394-F565-4A08-89D8-1AF8DCF4F61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99F2FC38-2D6B-4273-A901-6213E6DED4EC}"/>
   <bookViews>
-    <workbookView xWindow="8295" yWindow="2625" windowWidth="20550" windowHeight="11835" xr2:uid="{0DF55CA2-8073-418B-B7FF-723FBF917B41}"/>
+    <workbookView xWindow="6555" yWindow="2370" windowWidth="20550" windowHeight="11835" xr2:uid="{0DF55CA2-8073-418B-B7FF-723FBF917B41}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Waffle A (16)</t>
   </si>
@@ -74,9 +74,6 @@
     <t>high parasitics</t>
   </si>
   <si>
-    <t>low cap</t>
-  </si>
-  <si>
     <t>In layer</t>
   </si>
   <si>
@@ -147,6 +144,16 @@
   </si>
   <si>
     <t>Gesamt-Cap</t>
+  </si>
+  <si>
+    <t>low cap
+high var</t>
+  </si>
+  <si>
+    <t>high var</t>
+  </si>
+  <si>
+    <t>higher area/cap</t>
   </si>
 </sst>
 </file>
@@ -196,12 +203,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -216,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -244,6 +257,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -606,7 +623,7 @@
         <xdr:cNvPr id="8" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE5B1E6-6EF0-BE7E-F035-39E8ECA89C0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -935,7 +952,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,12 +964,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -970,13 +987,13 @@
       <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>32</v>
+      <c r="I1" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="8">
         <v>41</v>
@@ -1005,7 +1022,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2">
         <v>9.18</v>
@@ -1034,7 +1051,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -1058,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1066,12 +1083,12 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2">
         <v>54.98</v>
@@ -1087,7 +1104,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>59.74</v>
@@ -1116,7 +1133,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>57.53</v>
@@ -1138,12 +1155,12 @@
         <v>36.159999999999997</v>
       </c>
       <c r="I9" s="2">
-        <v>32.39</v>
+        <v>32.51</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
         <v>56.42</v>
@@ -1165,12 +1182,12 @@
         <v>34.909999999999997</v>
       </c>
       <c r="I10" s="2">
-        <v>31.2</v>
+        <v>31.19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
         <v>55.85</v>
@@ -1194,7 +1211,7 @@
         <v>34.299999999999997</v>
       </c>
       <c r="I11" s="2">
-        <v>30.55</v>
+        <v>30.59</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1209,7 +1226,7 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1221,7 +1238,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3">
         <v>573</v>
@@ -1239,7 +1256,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3">
         <v>574</v>
@@ -1257,18 +1274,21 @@
         <v>46.4</v>
       </c>
       <c r="G15" s="3">
-        <v>134</v>
+        <f t="shared" ref="G15:H15" si="0">1000*G8/48</f>
+        <v>133.95833333333334</v>
       </c>
       <c r="H15" s="3">
-        <v>694.5</v>
+        <f t="shared" si="0"/>
+        <v>694.58333333333337</v>
       </c>
       <c r="I15" s="3">
-        <v>621</v>
+        <f>1000*I8/48</f>
+        <v>621.25</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3">
         <v>575</v>
@@ -1284,18 +1304,21 @@
         <v>47.2</v>
       </c>
       <c r="G16" s="3">
-        <v>136.9</v>
+        <f t="shared" ref="G16:H16" si="1">1000*G9/52</f>
+        <v>136.92307692307693</v>
       </c>
       <c r="H16" s="3">
-        <v>695.3</v>
+        <f t="shared" si="1"/>
+        <v>695.38461538461536</v>
       </c>
       <c r="I16" s="3">
-        <v>622</v>
+        <f>1000*I9/52</f>
+        <v>625.19230769230762</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3">
         <v>576</v>
@@ -1311,18 +1334,21 @@
         <v>47.8</v>
       </c>
       <c r="G17" s="3">
+        <f t="shared" ref="G17:H17" si="2">1000*G10/50</f>
         <v>138.19999999999999</v>
       </c>
       <c r="H17" s="3">
+        <f t="shared" si="2"/>
         <v>698.2</v>
       </c>
       <c r="I17" s="3">
-        <v>624</v>
+        <f>1000*I10/50</f>
+        <v>623.79999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3">
         <v>576</v>
@@ -1340,13 +1366,16 @@
         <v>48</v>
       </c>
       <c r="G18" s="3">
-        <v>138.4</v>
+        <f t="shared" ref="G18:H18" si="3">1000*G11/49</f>
+        <v>138.36734693877551</v>
       </c>
       <c r="H18" s="3">
+        <f t="shared" si="3"/>
         <v>700</v>
       </c>
       <c r="I18" s="3">
-        <v>623.5</v>
+        <f>1000*I11/49</f>
+        <v>624.28571428571433</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1361,7 +1390,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1373,7 +1402,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="3">
         <f>B7/6/16*1000</f>
@@ -1391,7 +1420,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3">
         <f>(B8-B$7)/8*1000</f>
@@ -1407,7 +1436,7 @@
         <v>389.375</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" ref="F22" si="0">(F8-F$7)/8*1000</f>
+        <f t="shared" ref="F22" si="4">(F8-F$7)/8*1000</f>
         <v>51.250000000000014</v>
       </c>
       <c r="G22" s="6">
@@ -1425,7 +1454,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="3">
         <f>(B9-B$7)/4*1000</f>
@@ -1441,7 +1470,7 @@
         <v>384.99999999999977</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" ref="F23" si="1">(F9-F$7)/4*1000</f>
+        <f t="shared" ref="F23" si="5">(F9-F$7)/4*1000</f>
         <v>74.999999999999957</v>
       </c>
       <c r="G23" s="6">
@@ -1454,12 +1483,12 @@
       </c>
       <c r="I23" s="3">
         <f>(I9-I$8)/4*1000</f>
-        <v>642.50000000000011</v>
+        <v>672.49999999999943</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="3">
         <f>(B10-B$7)/2*1000</f>
@@ -1488,12 +1517,12 @@
       </c>
       <c r="I24" s="3">
         <f>(I10-I$8)/2*1000</f>
-        <v>689.99999999999955</v>
+        <v>685.00000000000045</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="3">
         <f>(B11-B$7)/1*1000</f>
@@ -1522,7 +1551,7 @@
       </c>
       <c r="I25" s="3">
         <f>(I11-I$8)/1*1000</f>
-        <v>730.00000000000045</v>
+        <v>769.99999999999955</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1545,23 +1574,27 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="3"/>
+      <c r="F28" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>

</xml_diff>